<commit_message>
ApachePOI - Cucumber 1
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu3\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu4\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulkemis11</t>
-  </si>
-  <si>
-    <t>ulkemis22</t>
-  </si>
-  <si>
-    <t>ulkemis33</t>
-  </si>
-  <si>
-    <t>ulkemis44</t>
-  </si>
-  <si>
-    <t>ulkemis55</t>
-  </si>
-  <si>
-    <t>ulkemis66</t>
-  </si>
-  <si>
-    <t>ulkemis77</t>
-  </si>
-  <si>
-    <t>ulkemis88</t>
-  </si>
-  <si>
-    <t>uis11</t>
-  </si>
-  <si>
-    <t>uis21</t>
-  </si>
-  <si>
-    <t>uis31</t>
-  </si>
-  <si>
-    <t>uis41</t>
-  </si>
-  <si>
-    <t>uis51</t>
-  </si>
-  <si>
-    <t>uis61</t>
-  </si>
-  <si>
-    <t>uis71</t>
-  </si>
-  <si>
-    <t>uis81</t>
+    <t>ulkemb3is11</t>
+  </si>
+  <si>
+    <t>ulkemb3is12</t>
+  </si>
+  <si>
+    <t>ulkemb3is13</t>
+  </si>
+  <si>
+    <t>ulkemb3is14</t>
+  </si>
+  <si>
+    <t>ulkemb3is15</t>
+  </si>
+  <si>
+    <t>ulkemb3is16</t>
+  </si>
+  <si>
+    <t>ulkemb3is17</t>
+  </si>
+  <si>
+    <t>ulkemb3is18</t>
+  </si>
+  <si>
+    <t>ub3is11</t>
+  </si>
+  <si>
+    <t>ub3is12</t>
+  </si>
+  <si>
+    <t>ub3is13</t>
+  </si>
+  <si>
+    <t>ub3is14</t>
+  </si>
+  <si>
+    <t>ub3is15</t>
+  </si>
+  <si>
+    <t>ub3is16</t>
+  </si>
+  <si>
+    <t>ub3is17</t>
+  </si>
+  <si>
+    <t>ub3is18</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="B1" sqref="B1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>